<commit_message>
update untuk menghilangkan auth
</commit_message>
<xml_diff>
--- a/public/Ticket Finish.xlsx
+++ b/public/Ticket Finish.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\i-mirs\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEEBFB4-EBBE-4A76-89E2-37F35CC2F392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E02B9B-A08A-43B5-AF66-8384DF6A09F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Sheet1!$A$13:$H$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Sheet1!$B$2:$I$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -373,13 +373,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -907,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F1BF87-762F-440D-88CA-B1BF3A57C479}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:H4"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2"/>
@@ -939,12 +939,12 @@
     </row>
     <row r="3" spans="1:9" ht="15.6" customHeight="1">
       <c r="B3" s="6"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="16.2" customHeight="1">
@@ -1141,14 +1141,14 @@
     </row>
     <row r="16" spans="1:9" ht="16.2" customHeight="1">
       <c r="B16" s="6"/>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="2:9">
@@ -1466,12 +1466,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D13:H13"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="D14:H14"/>
     <mergeCell ref="D15:H15"/>
@@ -1480,6 +1474,12 @@
     <mergeCell ref="D6:H6"/>
     <mergeCell ref="D7:H7"/>
     <mergeCell ref="D8:H8"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D13:H13"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.25" bottom="0.75" header="0.27" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>